<commit_message>
se modifico controlador excel
</commit_message>
<xml_diff>
--- a/public/excels/prueba1.xlsx
+++ b/public/excels/prueba1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>ITEM/RU</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>sj</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -443,15 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +522,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1699444</v>
       </c>
@@ -583,11 +586,8 @@
       <c r="U2">
         <v>7</v>
       </c>
-      <c r="V2">
-        <v>8</v>
-      </c>
-      <c r="W2">
-        <v>9</v>
+      <c r="V2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>